<commit_message>
add excel util add poiji
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CreateUserData.xlsx
+++ b/src/test/resources/testdata/CreateUserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\CommonRestAPIAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A412E1-9771-43BD-BB53-DDAA3407AFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E14F2C4-DCA3-40D7-A541-E0E4A8076168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>userName</t>
   </si>
@@ -33,16 +33,13 @@
     <t>password</t>
   </si>
   <si>
-    <t>Vinh Duong</t>
-  </si>
-  <si>
     <t>Helloworld1</t>
   </si>
   <si>
-    <t>Foden Duong</t>
-  </si>
-  <si>
     <t>Helloworld2</t>
+  </si>
+  <si>
+    <t>Random</t>
   </si>
 </sst>
 </file>
@@ -363,10 +360,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -378,10 +379,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -389,7 +390,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>